<commit_message>
Removed unnecessary test resources; tes package gen fixes
</commit_message>
<xml_diff>
--- a/tooling/src/test/resources/casereporting/tes/TES_Condition_Groupers_20240920.xlsx
+++ b/tooling/src/test/resources/casereporting/tes/TES_Condition_Groupers_20240920.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Adam/Src/cqframework/cqf-tooling/tooling/src/test/resources/casereporting/tes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Adam/Src/DBCG/aphl-tes/TESPackageGeneratorWorkspace/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFAFFF8E-EA29-464D-AB19-3E4805A68C41}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC67B0AE-13DB-EC41-997E-F380A7C5B83A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34200" windowHeight="20140" xr2:uid="{8F049818-7B3D-477B-AF9E-638E5733A0B8}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="503">
   <si>
     <t>Counter</t>
   </si>
@@ -1654,7 +1654,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1842,7 +1842,97 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note 2" xfId="4" xr:uid="{C78AD4B6-6D9F-47C5-ABC2-BD088B01CFE6}"/>
   </cellStyles>
-  <dxfs count="80">
+  <dxfs count="89">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2978,9 +3068,9 @@
   </sheetPr>
   <dimension ref="A1:F243"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A64" sqref="A64:XFD66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="37.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -7853,134 +7943,134 @@
   </sheetData>
   <autoFilter ref="A1:F243" xr:uid="{E87ADB4B-341B-4F2A-820B-D59071FEE9C7}"/>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="76" priority="102"/>
+    <cfRule type="duplicateValues" dxfId="88" priority="102"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B43 B46:B1048576">
-    <cfRule type="duplicateValues" dxfId="75" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="87" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="74" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="86" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B67 B71:B73">
-    <cfRule type="duplicateValues" dxfId="73" priority="55"/>
+    <cfRule type="duplicateValues" dxfId="85" priority="55"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B77:B84">
-    <cfRule type="duplicateValues" dxfId="72" priority="49"/>
-    <cfRule type="duplicateValues" dxfId="71" priority="50"/>
-    <cfRule type="duplicateValues" dxfId="70" priority="51"/>
-    <cfRule type="duplicateValues" dxfId="69" priority="52"/>
-    <cfRule type="duplicateValues" dxfId="68" priority="53"/>
+    <cfRule type="duplicateValues" dxfId="84" priority="49"/>
+    <cfRule type="duplicateValues" dxfId="83" priority="50"/>
+    <cfRule type="duplicateValues" dxfId="82" priority="51"/>
+    <cfRule type="duplicateValues" dxfId="81" priority="52"/>
+    <cfRule type="duplicateValues" dxfId="80" priority="53"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B101:B107">
-    <cfRule type="duplicateValues" dxfId="67" priority="44"/>
-    <cfRule type="duplicateValues" dxfId="66" priority="45"/>
-    <cfRule type="duplicateValues" dxfId="65" priority="46"/>
-    <cfRule type="duplicateValues" dxfId="64" priority="47"/>
-    <cfRule type="duplicateValues" dxfId="63" priority="48"/>
+    <cfRule type="duplicateValues" dxfId="79" priority="44"/>
+    <cfRule type="duplicateValues" dxfId="78" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="77" priority="46"/>
+    <cfRule type="duplicateValues" dxfId="76" priority="47"/>
+    <cfRule type="duplicateValues" dxfId="75" priority="48"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B110">
-    <cfRule type="duplicateValues" dxfId="62" priority="39"/>
-    <cfRule type="duplicateValues" dxfId="61" priority="40"/>
-    <cfRule type="duplicateValues" dxfId="60" priority="41"/>
-    <cfRule type="duplicateValues" dxfId="59" priority="42"/>
-    <cfRule type="duplicateValues" dxfId="58" priority="43"/>
+    <cfRule type="duplicateValues" dxfId="74" priority="39"/>
+    <cfRule type="duplicateValues" dxfId="73" priority="40"/>
+    <cfRule type="duplicateValues" dxfId="72" priority="41"/>
+    <cfRule type="duplicateValues" dxfId="71" priority="42"/>
+    <cfRule type="duplicateValues" dxfId="70" priority="43"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B123:B125">
-    <cfRule type="duplicateValues" dxfId="57" priority="34"/>
-    <cfRule type="duplicateValues" dxfId="56" priority="35"/>
-    <cfRule type="duplicateValues" dxfId="55" priority="36"/>
-    <cfRule type="duplicateValues" dxfId="54" priority="37"/>
-    <cfRule type="duplicateValues" dxfId="53" priority="38"/>
+    <cfRule type="duplicateValues" dxfId="69" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="68" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="67" priority="36"/>
+    <cfRule type="duplicateValues" dxfId="66" priority="37"/>
+    <cfRule type="duplicateValues" dxfId="65" priority="38"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B130:B132">
-    <cfRule type="duplicateValues" dxfId="52" priority="29"/>
-    <cfRule type="duplicateValues" dxfId="51" priority="30"/>
-    <cfRule type="duplicateValues" dxfId="50" priority="31"/>
-    <cfRule type="duplicateValues" dxfId="49" priority="32"/>
-    <cfRule type="duplicateValues" dxfId="48" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="64" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="63" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="62" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="61" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="60" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B142:B144">
-    <cfRule type="duplicateValues" dxfId="47" priority="24"/>
-    <cfRule type="duplicateValues" dxfId="46" priority="25"/>
-    <cfRule type="duplicateValues" dxfId="45" priority="26"/>
-    <cfRule type="duplicateValues" dxfId="44" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="59" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="58" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="57" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="56" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B143:B144">
-    <cfRule type="duplicateValues" dxfId="43" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="55" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B147:B149">
-    <cfRule type="duplicateValues" dxfId="42" priority="19"/>
-    <cfRule type="duplicateValues" dxfId="41" priority="20"/>
-    <cfRule type="duplicateValues" dxfId="40" priority="21"/>
-    <cfRule type="duplicateValues" dxfId="39" priority="22"/>
-    <cfRule type="duplicateValues" dxfId="38" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="54" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="53" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="52" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="51" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="50" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B152:B161">
-    <cfRule type="duplicateValues" dxfId="37" priority="13"/>
-    <cfRule type="duplicateValues" dxfId="36" priority="15"/>
-    <cfRule type="duplicateValues" dxfId="35" priority="16"/>
-    <cfRule type="duplicateValues" dxfId="34" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="49" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="48" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="46" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B153:B154 B156:B160">
-    <cfRule type="duplicateValues" dxfId="33" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="45" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B161">
-    <cfRule type="duplicateValues" dxfId="32" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="44" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B171:B174">
-    <cfRule type="duplicateValues" dxfId="31" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B172:B174">
-    <cfRule type="duplicateValues" dxfId="30" priority="199"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="199"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B177:B179">
-    <cfRule type="duplicateValues" dxfId="29" priority="3"/>
-    <cfRule type="duplicateValues" dxfId="28" priority="4"/>
-    <cfRule type="duplicateValues" dxfId="27" priority="5"/>
-    <cfRule type="duplicateValues" dxfId="26" priority="6"/>
-    <cfRule type="duplicateValues" dxfId="25" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B155:C155">
-    <cfRule type="duplicateValues" dxfId="24" priority="107"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="107"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="23" priority="100"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="100"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C6">
-    <cfRule type="duplicateValues" dxfId="22" priority="109"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="109"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:C47">
-    <cfRule type="duplicateValues" dxfId="21" priority="108"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="108"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C101:C1048576 C1:C99">
-    <cfRule type="duplicateValues" dxfId="20" priority="111"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="111"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C161 C70">
-    <cfRule type="duplicateValues" dxfId="19" priority="106"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="106"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C162:C163">
-    <cfRule type="duplicateValues" dxfId="18" priority="105"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="105"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C189">
-    <cfRule type="duplicateValues" dxfId="17" priority="104"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="104"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C228">
-    <cfRule type="duplicateValues" dxfId="16" priority="110"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="110"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C243:C1048576 C224:C229 C101:C221 C1:C99">
-    <cfRule type="duplicateValues" dxfId="15" priority="112"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="112"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C243:C1048576 C229 C224:C226 C1:C25 C188:C189 C101:C182 C27:C99">
-    <cfRule type="duplicateValues" dxfId="14" priority="113"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="113"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C243:C1048576 C229 C226 C1:C2 C7:C18 C20:C25 C27:C29 C143:C144 C146:C151 C153:C154 C156:C160 C167 C170 C172:C179 C31:C45 C101:C141 C48:C99 C164:C165">
-    <cfRule type="duplicateValues" dxfId="13" priority="168"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="168"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D206:D1048576 D101:D204 D1:D99">
-    <cfRule type="duplicateValues" dxfId="12" priority="103"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="103"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E101:E1048576 E1:E99">
-    <cfRule type="duplicateValues" dxfId="11" priority="101"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="101"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -7992,11 +8082,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="37.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -8031,19 +8121,19 @@
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1">
       <c r="A2" s="2">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2">
-        <v>89369001</v>
-      </c>
-      <c r="E2" s="24" t="s">
-        <v>6</v>
+        <v>132</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D2" s="4">
+        <v>715174007</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>134</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>7</v>
@@ -8051,59 +8141,99 @@
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1">
       <c r="A3" s="2">
-        <v>81</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>210</v>
+        <v>31</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="D3" s="2">
-        <v>81004002</v>
-      </c>
-      <c r="E3" s="24" t="s">
-        <v>211</v>
+        <v>135</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>137</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" customHeight="1">
+      <c r="A4" s="2">
+        <v>32</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" s="4">
+        <v>726492000</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F3" xr:uid="{E87ADB4B-341B-4F2A-820B-D59071FEE9C7}"/>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="79" priority="53"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="62"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="78" priority="1"/>
+  <conditionalFormatting sqref="B1 B5:B1048576">
+    <cfRule type="duplicateValues" dxfId="21" priority="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="77" priority="51"/>
+  <conditionalFormatting sqref="C1 C5:C1048576">
+    <cfRule type="duplicateValues" dxfId="20" priority="60"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="10" priority="239"/>
+  <conditionalFormatting sqref="B1 B5:B1048576">
+    <cfRule type="duplicateValues" dxfId="19" priority="248"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="9" priority="248"/>
+  <conditionalFormatting sqref="C1 C5:C1048576">
+    <cfRule type="duplicateValues" dxfId="18" priority="257"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="duplicateValues" dxfId="8" priority="251"/>
+  <conditionalFormatting sqref="E1 E5:E1048576">
+    <cfRule type="duplicateValues" dxfId="17" priority="260"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="7" priority="254"/>
-    <cfRule type="duplicateValues" dxfId="6" priority="255"/>
-    <cfRule type="duplicateValues" dxfId="5" priority="256"/>
-    <cfRule type="duplicateValues" dxfId="4" priority="257"/>
-    <cfRule type="duplicateValues" dxfId="3" priority="258"/>
+  <conditionalFormatting sqref="C1 C5:C1048576">
+    <cfRule type="duplicateValues" dxfId="11" priority="271"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="262"/>
+  <conditionalFormatting sqref="C1 C5:C1048576">
+    <cfRule type="duplicateValues" dxfId="10" priority="274"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="265"/>
+  <conditionalFormatting sqref="D1 D5:D1048576">
+    <cfRule type="duplicateValues" dxfId="9" priority="277"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="268"/>
+  <conditionalFormatting sqref="B2:B4">
+    <cfRule type="duplicateValues" dxfId="8" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B4">
+    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C4">
+    <cfRule type="duplicateValues" dxfId="6" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C4">
+    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C4">
+    <cfRule type="duplicateValues" dxfId="4" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C4">
+    <cfRule type="duplicateValues" dxfId="3" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C4">
+    <cfRule type="duplicateValues" dxfId="2" priority="9"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D4">
+    <cfRule type="duplicateValues" dxfId="1" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E4">
+    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -8111,26 +8241,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="2748ded2-c890-4c13-80b9-352cbe63b876" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ababbff0-3a86-4f6a-a1e2-ba6807a807ae">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010035415D7933C1644FA0B7A1B0E6079AD3" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="02dd4851cb9e04cf7bc8246dda28a3ce">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ababbff0-3a86-4f6a-a1e2-ba6807a807ae" xmlns:ns3="2748ded2-c890-4c13-80b9-352cbe63b876" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="36bcb32edc274f382221f14415603a2e" ns2:_="" ns3:_="">
     <xsd:import namespace="ababbff0-3a86-4f6a-a1e2-ba6807a807ae"/>
@@ -8359,10 +8469,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="2748ded2-c890-4c13-80b9-352cbe63b876" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ababbff0-3a86-4f6a-a1e2-ba6807a807ae">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{451912C6-DC3C-4651-B926-C8A07E4AFAA9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB164146-BB73-432A-8088-4E3DA61BB1B3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ababbff0-3a86-4f6a-a1e2-ba6807a807ae"/>
+    <ds:schemaRef ds:uri="2748ded2-c890-4c13-80b9-352cbe63b876"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8379,20 +8520,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB164146-BB73-432A-8088-4E3DA61BB1B3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{451912C6-DC3C-4651-B926-C8A07E4AFAA9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="ababbff0-3a86-4f6a-a1e2-ba6807a807ae"/>
-    <ds:schemaRef ds:uri="2748ded2-c890-4c13-80b9-352cbe63b876"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>